<commit_message>
Refatoração de fluxos corrompidos
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Documents\UiPath\CalculateClientSecurityHash\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB70F7CC-E9A2-4EEF-9D51-C9E40B59AD92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5198369-75CA-4011-ACEF-349ACD43720B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="45">
   <si>
     <t>Name</t>
   </si>
@@ -152,6 +152,12 @@
   </si>
   <si>
     <t>ACME_Credentials</t>
+  </si>
+  <si>
+    <t>System1_Url</t>
+  </si>
+  <si>
+    <t>https://acme-test.uipath.com/</t>
   </si>
 </sst>
 </file>
@@ -185,7 +191,7 @@
     <font>
       <u/>
       <sz val="11"/>
-      <color rgb="FF000000"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -207,8 +213,9 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -220,9 +227,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hiperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -613,11 +621,18 @@
       </c>
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A6" s="5"/>
+      <c r="A6" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="8" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="9" spans="1:26" ht="14.25" customHeight="1">
+      <c r="B9" s="2"/>
+    </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="12" spans="1:26" ht="14.25" customHeight="1"/>
@@ -1608,8 +1623,11 @@
     <row r="997" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
+  <hyperlinks>
+    <hyperlink ref="B6" r:id="rId1" xr:uid="{DFBCF3AD-C3AB-49D7-A06A-458BE10F47C9}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>